<commit_message>
Update ProvinicaController, fixed EscolaController and update on EscolaView.
</commit_message>
<xml_diff>
--- a/ExcelTeste.xlsx
+++ b/ExcelTeste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Nº</t>
   </si>
@@ -33,13 +33,31 @@
     <t>Província</t>
   </si>
   <si>
-    <t>Escola Técnica de Luanda</t>
-  </si>
-  <si>
-    <t>luanda.escola@gmail.com</t>
-  </si>
-  <si>
     <t>Luanda</t>
+  </si>
+  <si>
+    <t>Escola 20</t>
+  </si>
+  <si>
+    <t>Escola 21</t>
+  </si>
+  <si>
+    <t>Escola 22</t>
+  </si>
+  <si>
+    <t>escola20@gmail.com</t>
+  </si>
+  <si>
+    <t>Bié</t>
+  </si>
+  <si>
+    <t>Huambo</t>
+  </si>
+  <si>
+    <t>escola22@gmail.com</t>
+  </si>
+  <si>
+    <t>escola21@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -412,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,27 +465,51 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>233</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -577,8 +619,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>